<commit_message>
single choice excel template chages
</commit_message>
<xml_diff>
--- a/rmsapp.rmssysapi.service/Resources/UploadTemplates/RMSUploadTemplate-Quiz.xlsx
+++ b/rmsapp.rmssysapi.service/Resources/UploadTemplates/RMSUploadTemplate-Quiz.xlsx
@@ -35,16 +35,16 @@
     <t>Text_Answer(s)</t>
   </si>
   <si>
-    <t>Radio</t>
-  </si>
-  <si>
     <t>cd</t>
   </si>
   <si>
-    <t>Single Choice</t>
-  </si>
-  <si>
-    <t>Multiple Choice</t>
+    <t>SingleChoice</t>
+  </si>
+  <si>
+    <t>MultipleChoice</t>
+  </si>
+  <si>
+    <t>Programm</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A2:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +470,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -483,17 +483,17 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
       <formula1>QuestionType</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F5">
@@ -504,5 +504,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>